<commit_message>
work on #13 - frequency counts
</commit_message>
<xml_diff>
--- a/libchickadee/test/test_data/test_ips.xlsx
+++ b/libchickadee/test/test_data/test_ips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\dev\chickadee\libchickadee\test\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chapin/Documents/dev/chickadee/chickadee/libchickadee/test/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5998C5AB-2C46-4374-A43F-6F9F318B8FEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FC2F34-657B-9F4A-A3BB-9CCE1DCB938D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8310" yWindow="-14895" windowWidth="28110" windowHeight="11835" xr2:uid="{C10EC023-62D9-4F3D-A7F9-CF061E985C32}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{C10EC023-62D9-4F3D-A7F9-CF061E985C32}"/>
   </bookViews>
   <sheets>
     <sheet name="custom_tab1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>2001:4860:4860::8844</t>
   </si>
@@ -406,33 +406,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9333FE-1417-4D5C-AC41-2959D9BB6202}">
   <dimension ref="A2:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -444,25 +444,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7AA278-C949-4D02-A08E-6B8822E298C1}">
-  <dimension ref="G9:G16"/>
+  <dimension ref="B9:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="E14:F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="9" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
         <v>6</v>
       </c>

</xml_diff>